<commit_message>
actualizacion documento de Bugs
</commit_message>
<xml_diff>
--- a/ITERACION 5/SUB ITERACION 5/CASOS DE PRUEBA/PlantillaPropuestaResultadoBugs_CP_SI_CUS.xlsx
+++ b/ITERACION 5/SUB ITERACION 5/CASOS DE PRUEBA/PlantillaPropuestaResultadoBugs_CP_SI_CUS.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="30" windowWidth="12915" windowHeight="7740" activeTab="5"/>
@@ -14,12 +14,12 @@
     <sheet name="SI_CUS014" sheetId="5" r:id="rId5"/>
     <sheet name="SI_CUS015" sheetId="1" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="114210"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="28">
   <si>
     <t>IDBug</t>
   </si>
@@ -132,12 +132,64 @@
   <si>
     <t>1. El sistema guarda el registro actualizado. Sin embargo al volver a listar los Procesos en el campo Responsable no se muestra el valor modificado</t>
   </si>
+  <si>
+    <t>TC1_SI_CUS014</t>
+  </si>
+  <si>
+    <t>1. Seleccionar la opción del menú "Crear Proceso" de la interfaz principal.
+2. El sistema muestra la interfaz "Crear Procesos" donde se visualizan las listas desplegables de tipo de proceso, responsable, MTD, RTO, prioridad correspondiente a los impactos de imagen, operativo, económico, regulatorio o contractual e imagen, y las cajas de texto para ingresar el nombre y objetivo del proceso.
+3. Ingresar el nombre del proceso.
+4. Ingresar el objetivo del proceso.
+5. Seleccionar un elemento de la lista "Tipo Proceso".
+6. Seleccionar un elemento de la lista "Responsable".
+7. Seleccionar un elemento de la lista "MTD".
+8. Seleccionar un elemento de la lista "RTO".
+9.  Seleccionar un elemento de la lista "Prioridad del Impacto Imagen".
+10. Seleccionar un elemento de la lista "Prioridad del Impacto Operativo".
+11. Seleccionar un elemento de la lista "Prioridad del Impacto Económico".
+12. Seleccionar un elemento de la lista "Prioridad del Impacto Regulatorio o Contractual".
+13. Seleccionar un elemento de la lista "Prioridad del Impacto Imagen".
+14. Dar clic sobre botón "Registrar Proceso".</t>
+  </si>
+  <si>
+    <t>1. Seleccionar la opción del menú "Crear Proceso" de la interfaz principal.
+2. El sistema muestra la interfaz "Crear Procesos" donde se visualizan las listas desplegables de tipo de proceso, responsable, MTD, RTO, prioridad correspondiente a los impactos de imagen, operativo, económico, regulatorio o contractual e imagen, y las cajas de texto para ingresar el nombre y objetivo del proceso.
+3. Ingresar el nombre del proceso.
+4. No ingresar el objetivo del proceso.
+5. Seleccionar un elemento de la lista "Tipo Proceso".
+6. Seleccionar un elemento de la lista "Responsable".
+7. Seleccionar un elemento de la lista "MTD".
+8. Seleccionar un elemento de la lista "RTO".
+9.  Seleccionar un elemento de la lista "Prioridad del Impacto Imagen".
+10. Seleccionar un elemento de la lista "Prioridad del Impacto Operativo".
+11. Seleccionar un elemento de la lista "Prioridad del Impacto Económico".
+12. Seleccionar un elemento de la lista "Prioridad del Impacto Regulatorio o Contractual".
+13. Seleccionar un elemento de la lista "Prioridad del Impacto Imagen".
+14. Dar clic sobre botón "Registrar Proceso".</t>
+  </si>
+  <si>
+    <t>1. En el menú no figura la opción "Crear Proceso" sino "Creacion de Procesos".
+2. El sistema no muestra la interfaz "Crear Procesos" sino "Registrar Proceso".
+3. La interfaz muestra por duplicado la lista desplegable "Proridad del Impacto Imagen".
+4. El sistema muestra un mensaje de notificación, indicando que el registro fue grabado con éxito.
+5. El sistema no limpia las listas despegables de prioridad correspondiente a los impactos de imagen, operativo, económico, regulatorio o contractual e imagen del formulario.</t>
+  </si>
+  <si>
+    <t>1. El menú debe mostrar la opción "Creacion de Procesos". 
+2. El sistema debe mostrar la interfaz "Registrar Proceso". 
+3. La interfaz debe mostrar la lista despegable "Proridad del Impacto Imagen" una sola vez. 
+4. El sistema muestra un mensaje de notificación, indicando que el registro fue grabado con éxito.
+5. El sistema debe limpiar los campos del formulario sin excepción.</t>
+  </si>
+  <si>
+    <t>Duplidad de datos</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,10 +200,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -226,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -240,21 +296,18 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -263,16 +316,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -346,7 +394,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -381,7 +428,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -557,14 +603,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <tabColor indexed="46"/>
+  </sheetPr>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.85546875" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
@@ -575,7 +624,7 @@
     <col min="7" max="7" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -595,7 +644,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="360" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="360">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -616,7 +665,63 @@
       </c>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="225">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -626,7 +731,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -636,7 +741,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -646,7 +751,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -657,21 +762,22 @@
       <c r="F6" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -691,7 +797,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="225" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="225">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -711,7 +817,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -721,7 +827,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -731,7 +837,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -741,7 +847,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -752,21 +858,22 @@
       <c r="F6" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -786,7 +893,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="225" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="225">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -806,7 +913,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -816,7 +923,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -826,7 +933,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -836,7 +943,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -847,21 +954,31 @@
       <c r="F6" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <tabColor indexed="57"/>
+  </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F6"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="4" max="4" width="49.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -881,37 +998,39 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="225" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="398.25" customHeight="1">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="390">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -921,7 +1040,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -931,7 +1050,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -942,114 +1061,29 @@
       <c r="F6" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="225" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <tabColor indexed="45"/>
+  </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="22.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
@@ -1058,7 +1092,7 @@
     <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1078,27 +1112,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="409.5">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="409.5">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1107,20 +1141,20 @@
       <c r="D3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="1:6" ht="409.5">
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
       <c r="D4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1129,6 +1163,7 @@
     <mergeCell ref="F2:F4"/>
     <mergeCell ref="E2:E4"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>